<commit_message>
First draft of CapabilityStatement (lots more to do)
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-CEQSubscriptionBundle.xlsx
+++ b/output/StructureDefinition-CEQSubscriptionBundle.xlsx
@@ -6960,7 +6960,7 @@
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F55" t="s" s="2">
         <v>49</v>
@@ -10488,7 +10488,7 @@
       </c>
       <c r="D87" s="2"/>
       <c r="E87" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F87" t="s" s="2">
         <v>49</v>

</xml_diff>

<commit_message>
Fix non-use of us-core-org
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-CEQSubscriptionBundle.xlsx
+++ b/output/StructureDefinition-CEQSubscriptionBundle.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5027" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5027" uniqueCount="250">
   <si>
     <t>Path</t>
   </si>
@@ -772,8 +772,24 @@
     <t>subserv</t>
   </si>
   <si>
-    <t xml:space="preserve">Organization
+    <t xml:space="preserve">Organization {http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization}
 </t>
+  </si>
+  <si>
+    <t>A grouping of people or organizations with a common purpose</t>
+  </si>
+  <si>
+    <t>A formally or informally recognized grouping of people or organizations formed for the purpose of achieving some form of collective action.  Includes companies, institutions, corporations, departments, community groups, healthcare practice groups, payer/insurer, etc.</t>
+  </si>
+  <si>
+    <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}org-1:The organization SHALL at least have a name or an identifier, and possibly more than one {(identifier.count() + name.count()) &gt; 0}</t>
+  </si>
+  <si>
+    <t>(also see master files messages)</t>
+  </si>
+  <si>
+    <t>Organization(classCode=ORG, determinerCode=INST)</t>
   </si>
   <si>
     <t>Bundle.signature</t>
@@ -985,8 +1001,8 @@
     <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="25.01171875" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="22.671875" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="29.51171875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="48.6640625" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="41.4296875" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="32.84375" customWidth="true" bestFit="true"/>
   </cols>
@@ -14035,16 +14051,16 @@
         <v>40</v>
       </c>
       <c r="I119" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J119" t="s" s="2">
         <v>238</v>
       </c>
       <c r="K119" t="s" s="2">
-        <v>156</v>
+        <v>239</v>
       </c>
       <c r="L119" t="s" s="2">
-        <v>157</v>
+        <v>240</v>
       </c>
       <c r="M119" s="2"/>
       <c r="N119" s="2"/>
@@ -14107,13 +14123,13 @@
         <v>40</v>
       </c>
       <c r="AI119" t="s" s="2">
-        <v>40</v>
+        <v>241</v>
       </c>
       <c r="AJ119" t="s" s="2">
-        <v>40</v>
+        <v>242</v>
       </c>
       <c r="AK119" t="s" s="2">
-        <v>40</v>
+        <v>243</v>
       </c>
       <c r="AL119" t="s" s="2">
         <v>40</v>
@@ -16879,7 +16895,7 @@
     </row>
     <row r="145" hidden="true">
       <c r="A145" t="s" s="2">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" t="s" s="2">
@@ -16902,19 +16918,19 @@
         <v>50</v>
       </c>
       <c r="J145" t="s" s="2">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="K145" t="s" s="2">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="L145" t="s" s="2">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="M145" t="s" s="2">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="N145" t="s" s="2">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="O145" t="s" s="2">
         <v>40</v>
@@ -16963,7 +16979,7 @@
         <v>40</v>
       </c>
       <c r="AE145" t="s" s="2">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="AF145" t="s" s="2">
         <v>41</v>

</xml_diff>